<commit_message>
Update Gantt And Add Apresentacao
</commit_message>
<xml_diff>
--- a/documentacao/Planilha - Gantt.xlsx
+++ b/documentacao/Planilha - Gantt.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E3F2DAA-A5A8-44FB-A160-08AD7CA3BCED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EB9C89C-033F-4692-AA74-E6EAE4C76E2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="1" activeTab="1" xr2:uid="{83E43DC8-C7A0-4A4D-AAF4-DA46DABAE971}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2400" windowHeight="585" firstSheet="1" activeTab="1" xr2:uid="{83E43DC8-C7A0-4A4D-AAF4-DA46DABAE971}"/>
   </bookViews>
   <sheets>
     <sheet name="Controlador de Projetos" sheetId="4" r:id="rId1"/>
@@ -20,11 +20,12 @@
     <definedName name="IncrementoDeRolagem">Marcos[Posição]</definedName>
     <definedName name="InícioDoDia">Marcos[Início do dia]</definedName>
     <definedName name="Marco">Marcos[Marco/Atividade]</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Controlador de Projetos'!$4:$5</definedName>
     <definedName name="Rolagem">'Gráfico de Gantt'!$C$1</definedName>
     <definedName name="TabeladeDataInicial">Marcos[Data de Início]</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Controlador de Projetos'!$4:$5</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -237,7 +237,7 @@
     <numFmt numFmtId="166" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -949,59 +949,58 @@
     </xf>
   </cellXfs>
   <cellStyles count="48">
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="7" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="45" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="42" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="46" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="43" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="47" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="44" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="15" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="19" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="21" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Comma" xfId="6" builtinId="3" customBuiltin="1"/>
-    <cellStyle name="Comma [0]" xfId="9" builtinId="6" customBuiltin="1"/>
-    <cellStyle name="Currency" xfId="10" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Currency [0]" xfId="11" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase1" xfId="26" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase2" xfId="30" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase3" xfId="34" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase4" xfId="38" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase5" xfId="7" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Ênfase6" xfId="45" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase1" xfId="27" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase2" xfId="31" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase3" xfId="35" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase4" xfId="39" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase5" xfId="42" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Ênfase6" xfId="46" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase1" xfId="28" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase2" xfId="32" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase3" xfId="36" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase4" xfId="40" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase5" xfId="43" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Ênfase6" xfId="47" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bom" xfId="14" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="19" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Célula de Verificação" xfId="21" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Célula Vinculada" xfId="20" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Data" xfId="4" xr:uid="{A5654282-6065-4D12-BA7A-82AAEC707206}"/>
-    <cellStyle name="Explanatory Text" xfId="8" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="14" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="2" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="3" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="17" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="16" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Ênfase1" xfId="25" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Ênfase2" xfId="29" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Ênfase3" xfId="33" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Ênfase4" xfId="37" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Ênfase5" xfId="41" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Ênfase6" xfId="44" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="17" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Moeda" xfId="10" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Moeda [0]" xfId="11" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="Neutro" xfId="16" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Note" xfId="23" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="18" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Percent" xfId="12" builtinId="5" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="13" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Nota" xfId="23" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Porcentagem" xfId="12" builtinId="5" customBuiltin="1"/>
+    <cellStyle name="Ruim" xfId="15" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Saída" xfId="18" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Separador de milhares [0]" xfId="9" builtinId="6" customBuiltin="1"/>
+    <cellStyle name="Texto de Aviso" xfId="22" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto Explicativo" xfId="8" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="13" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 1" xfId="1" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="2" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="3" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="24" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="22" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Vírgula" xfId="6" builtinId="3" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="21">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left/>
         <right style="medium">
           <color theme="5" tint="-0.249977111117893"/>
@@ -1011,7 +1010,8 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <numFmt numFmtId="0" formatCode="General"/>
+      <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="medium">
           <color theme="5" tint="-0.249977111117893"/>
@@ -1027,6 +1027,16 @@
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="medium">
+          <color theme="5" tint="-0.249977111117893"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
@@ -1040,29 +1050,11 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="medium">
-          <color theme="5" tint="-0.249977111117893"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <bottom style="medium">
           <color theme="5" tint="-0.249977111117893"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1093,26 +1085,12 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color theme="4" tint="0.39994506668294322"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1155,6 +1133,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color theme="4" tint="0.39994506668294322"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1235,6 +1221,20 @@
         <bottom/>
       </border>
       <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1323,7 +1323,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="1" defaultPivotStyle="PivotStyleLight16">
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Estilo de tabela do Gráfico de Gantt" pivot="0" count="2" xr9:uid="{D7A9D309-76D4-47FD-AAFA-79E72526BC00}">
       <tableStyleElement type="headerRow" dxfId="20"/>
       <tableStyleElement type="firstRowStripe" dxfId="19"/>
@@ -1343,7 +1343,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1389,19 +1389,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Funcionalidade CSV</c:v>
+                  <c:v>Tela de cadastro</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Doc. API (SWAGGER)</c:v>
+                  <c:v>Interface WEB</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Desenho de Arq. alto nivel</c:v>
+                  <c:v>2CRUD(Spring + ORM)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Observer e Interator</c:v>
+                  <c:v>Planilha de arquitetura</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Diagrama Solução (Container)</c:v>
+                  <c:v>teste</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1416,16 +1416,16 @@
                   <c:v>44646</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44646</c:v>
+                  <c:v>44649</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>44646</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>44646</c:v>
+                  <c:v>44649</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>44646</c:v>
+                  <c:v>44657</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1466,19 +1466,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Funcionalidade CSV</c:v>
+                  <c:v>Tela de cadastro</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Doc. API (SWAGGER)</c:v>
+                  <c:v>Interface WEB</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Desenho de Arq. alto nivel</c:v>
+                  <c:v>2CRUD(Spring + ORM)</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Observer e Interator</c:v>
+                  <c:v>Planilha de arquitetura</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Diagrama Solução (Container)</c:v>
+                  <c:v>teste</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1490,19 +1490,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1560,7 +1560,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="746878512"/>
@@ -1618,7 +1618,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="746877856"/>
@@ -1666,7 +1666,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="pt-BR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2221,10 +2221,10 @@
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2262,16 +2262,16 @@
     <sortCondition ref="D6:D21"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="12" xr3:uid="{417148D6-7A28-40C6-80F2-B6C648F24A03}" name="Posição" totalsRowLabel="Total" dataDxfId="17" totalsRowDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{0B09DBBE-2FBF-46E2-8C69-E2CFCC08C5F9}" name="Data de Início" dataDxfId="15" totalsRowDxfId="16" dataCellStyle="Data"/>
-    <tableColumn id="3" xr3:uid="{5169FF04-1487-4814-B98C-C577FE120139}" name="Data de Término" dataDxfId="13" totalsRowDxfId="14" dataCellStyle="Data"/>
-    <tableColumn id="10" xr3:uid="{DBA6C66F-3413-4788-966C-44D320586126}" name="Marco/Atividade" dataDxfId="11" totalsRowDxfId="12">
+    <tableColumn id="12" xr3:uid="{417148D6-7A28-40C6-80F2-B6C648F24A03}" name="Posição" totalsRowLabel="Total" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{0B09DBBE-2FBF-46E2-8C69-E2CFCC08C5F9}" name="Data de Início" dataDxfId="16" totalsRowDxfId="15" dataCellStyle="Data"/>
+    <tableColumn id="3" xr3:uid="{5169FF04-1487-4814-B98C-C577FE120139}" name="Data de Término" dataDxfId="14" totalsRowDxfId="13" dataCellStyle="Data"/>
+    <tableColumn id="10" xr3:uid="{DBA6C66F-3413-4788-966C-44D320586126}" name="Marco/Atividade" dataDxfId="12" totalsRowDxfId="11">
       <calculatedColumnFormula>"Atividade"&amp;" "&amp;ROW($A1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{31798575-BD57-466D-AC99-9EF7707B63C7}" name="Início do dia" dataDxfId="9" totalsRowDxfId="10">
+    <tableColumn id="11" xr3:uid="{31798575-BD57-466D-AC99-9EF7707B63C7}" name="Início do dia" dataDxfId="10" totalsRowDxfId="9">
       <calculatedColumnFormula>IFERROR(IF(OR(LEN(Marcos[[#This Row],[Data de Início]])=0,LEN(Marcos[[#This Row],[Data de Término]])=0),"",INT(C6)-INT($C$6)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{A36515AD-389B-4321-BB8D-89BAC7740995}" name="Duração da tarefa" totalsRowFunction="count" dataDxfId="7" totalsRowDxfId="8">
+    <tableColumn id="8" xr3:uid="{A36515AD-389B-4321-BB8D-89BAC7740995}" name="Duração da tarefa" totalsRowFunction="count" dataDxfId="8" totalsRowDxfId="7">
       <calculatedColumnFormula>IFERROR(IF(Marcos[[#This Row],[Início do dia]]=0,DATEDIF(Marcos[[#This Row],[Data de Início]],Marcos[[#This Row],[Data de Término]],"d")+1,IF(LEN(Marcos[[#This Row],[Início do dia]])=0,"",DATEDIF(Marcos[[#This Row],[Data de Início]],Marcos[[#This Row],[Data de Término]],"d")+1)),0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2293,7 +2293,7 @@
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D75F8E51-B33E-49A6-911D-57AEC59F5557}" name="marco" totalsRowLabel="Total" dataDxfId="4" totalsRowDxfId="5">
+    <tableColumn id="1" xr3:uid="{D75F8E51-B33E-49A6-911D-57AEC59F5557}" name="marco" totalsRowLabel="Total" dataDxfId="5" totalsRowDxfId="4">
       <calculatedColumnFormula>IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$E6,Rolagem,0,1,1))=0,"",INDEX(Marcos[],'Controlador de Projetos'!$B6+Rolagem,4)),"")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{24BD43CB-1C65-4F2C-BE9D-D5C601681B07}" name="data" dataDxfId="3">
@@ -2302,7 +2302,7 @@
     <tableColumn id="3" xr3:uid="{1391FB0D-B504-4322-B211-D2B787F64A2D}" name="Início do dia" dataDxfId="2">
       <calculatedColumnFormula>IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$F6,Rolagem,0,1,1))=0,"",INDEX(Marcos[],'Controlador de Projetos'!$B6+Rolagem,5)),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{21D31F93-1DE3-4841-8614-466E50A648E8}" name="duração" totalsRowFunction="sum" dataDxfId="0" totalsRowDxfId="1">
+    <tableColumn id="4" xr3:uid="{21D31F93-1DE3-4841-8614-466E50A648E8}" name="duração" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0">
       <calculatedColumnFormula>IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$G6,Rolagem,0,1,1))=0,"",INDEX(Marcos[],'Controlador de Projetos'!$B6+Rolagem,6)),"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2587,7 +2587,7 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="14" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
@@ -2599,7 +2599,7 @@
     <col min="8" max="8" width="3.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="50.1" customHeight="1">
+    <row r="1" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -2607,7 +2607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1" thickBot="1">
+    <row r="2" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>44646</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="30" customHeight="1" thickBot="1">
+    <row r="3" spans="1:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
@@ -2632,7 +2632,7 @@
       </c>
       <c r="E3" s="12"/>
     </row>
-    <row r="4" spans="1:7" ht="105" customHeight="1">
+    <row r="4" spans="1:7" ht="105" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>6</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>13</v>
       </c>
@@ -2678,7 +2678,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="23">
         <v>1</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="23">
         <v>2</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="23">
         <v>3</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="23">
         <v>4</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="23">
         <v>5</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="23">
         <v>6</v>
       </c>
@@ -2812,7 +2812,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="23">
         <v>7</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="23">
         <v>8</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="23">
         <v>9</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="23">
         <v>10</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="23">
         <v>11</v>
       </c>
@@ -2926,7 +2926,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="23">
         <v>12</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="23">
         <v>13</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="23">
         <v>14</v>
       </c>
@@ -2994,7 +2994,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" s="23"/>
       <c r="C20" s="26"/>
       <c r="D20" s="26"/>
@@ -3008,7 +3008,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="25"/>
       <c r="C21" s="27"/>
       <c r="D21" s="27"/>
@@ -3022,7 +3022,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
         <v>34</v>
       </c>
@@ -3056,16 +3056,16 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.5703125" customWidth="1"/>
     <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="27.75" customHeight="1">
+    <row r="1" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>36</v>
       </c>
@@ -3073,11 +3073,11 @@
         <v>37</v>
       </c>
       <c r="C1" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="14.45" customHeight="1"/>
-    <row r="3" spans="1:3" ht="14.45" customHeight="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Incremento de rolagem" prompt="Alterar esse número rolará o Gráfico de Gantt." sqref="C1" xr:uid="{71F0885F-3AE1-4760-8878-DABCD535613C}"/>
@@ -3101,37 +3101,37 @@
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="78.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="50.1" customHeight="1">
+    <row r="1" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="50.1" customHeight="1">
+    <row r="2" spans="1:1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="180">
+    <row r="3" spans="1:1" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="255">
+    <row r="5" spans="1:1" ht="255" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>43</v>
       </c>
@@ -3155,7 +3155,7 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.5703125" style="14" customWidth="1"/>
     <col min="2" max="2" width="20.5703125" customWidth="1"/>
@@ -3164,7 +3164,7 @@
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="50.1" customHeight="1">
+    <row r="1" spans="1:6" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>44</v>
       </c>
@@ -3172,7 +3172,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>46</v>
       </c>
@@ -3180,7 +3180,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1">
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="14" t="s">
         <v>48</v>
       </c>
@@ -3200,10 +3200,10 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="6" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$E6,Rolagem,0,1,1))=0,"",INDEX(Marcos[],'Controlador de Projetos'!$B6+Rolagem,4)),"")</f>
-        <v>Funcionalidade CSV</v>
+        <v>Tela de cadastro</v>
       </c>
       <c r="C6" s="7">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$C6,Rolagem,0,1,1))=0,Data_de_término,INDEX(Marcos[],'Controlador de Projetos'!$B6+Rolagem,2)),"")</f>
@@ -3215,31 +3215,31 @@
       </c>
       <c r="E6" s="9">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$G6,Rolagem,0,1,1))=0,"",INDEX(Marcos[],'Controlador de Projetos'!$B6+Rolagem,6)),"")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="6" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$E7,Rolagem,0,1,1))=0,"",INDEX(Marcos[],'Controlador de Projetos'!$B7+Rolagem,4)),"")</f>
-        <v>Doc. API (SWAGGER)</v>
+        <v>Interface WEB</v>
       </c>
       <c r="C7" s="7">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$C7,Rolagem,0,1,1))=0,Data_de_término,INDEX(Marcos[],'Controlador de Projetos'!$B7+Rolagem,2)),"")</f>
-        <v>44646</v>
+        <v>44649</v>
       </c>
       <c r="D7" s="8">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$F7,Rolagem,0,1,1))=0,"",INDEX(Marcos[],'Controlador de Projetos'!$B7+Rolagem,5)),"")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E7" s="9">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$G7,Rolagem,0,1,1))=0,"",INDEX(Marcos[],'Controlador de Projetos'!$B7+Rolagem,6)),"")</f>
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1">
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$E8,Rolagem,0,1,1))=0,"",INDEX(Marcos[],'Controlador de Projetos'!$B8+Rolagem,4)),"")</f>
-        <v>Desenho de Arq. alto nivel</v>
+        <v>2CRUD(Spring + ORM)</v>
       </c>
       <c r="C8" s="7">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$C8,Rolagem,0,1,1))=0,Data_de_término,INDEX(Marcos[],'Controlador de Projetos'!$B8+Rolagem,2)),"")</f>
@@ -3251,43 +3251,43 @@
       </c>
       <c r="E8" s="9">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$G8,Rolagem,0,1,1))=0,"",INDEX(Marcos[],'Controlador de Projetos'!$B8+Rolagem,6)),"")</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="6" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$E9,Rolagem,0,1,1))=0,"",INDEX(Marcos[],'Controlador de Projetos'!$B9+Rolagem,4)),"")</f>
-        <v>Observer e Interator</v>
+        <v>Planilha de arquitetura</v>
       </c>
       <c r="C9" s="7">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$C9,Rolagem,0,1,1))=0,Data_de_término,INDEX(Marcos[],'Controlador de Projetos'!$B9+Rolagem,2)),"")</f>
-        <v>44646</v>
+        <v>44649</v>
       </c>
       <c r="D9" s="8">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$F9,Rolagem,0,1,1))=0,"",INDEX(Marcos[],'Controlador de Projetos'!$B9+Rolagem,5)),"")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E9" s="9">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$G9,Rolagem,0,1,1))=0,"",INDEX(Marcos[],'Controlador de Projetos'!$B9+Rolagem,6)),"")</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="str">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$E10,Rolagem,0,1,1))=0,"",INDEX(Marcos[],'Controlador de Projetos'!$B10+Rolagem,4)),"")</f>
-        <v>Diagrama Solução (Container)</v>
+        <v>teste</v>
       </c>
       <c r="C10" s="7">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$C10,Rolagem,0,1,1))=0,Data_de_término,INDEX(Marcos[],'Controlador de Projetos'!$B10+Rolagem,2)),"")</f>
-        <v>44646</v>
+        <v>44657</v>
       </c>
       <c r="D10" s="8">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$F10,Rolagem,0,1,1))=0,"",INDEX(Marcos[],'Controlador de Projetos'!$B10+Rolagem,5)),"")</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="E10" s="9">
         <f ca="1">IFERROR(IF(LEN(OFFSET('Controlador de Projetos'!$G10,Rolagem,0,1,1))=0,"",INDEX(Marcos[],'Controlador de Projetos'!$B10+Rolagem,6)),"")</f>
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>